<commit_message>
updated test data set
</commit_message>
<xml_diff>
--- a/dev/data.xlsx
+++ b/dev/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/Labs/Zhang/Lokki/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F414B9A0-1896-584E-A57C-E36D69C49F10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE1AFCE-094F-044B-8DA8-BF5D8974CE86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10580" yWindow="6100" windowWidth="27640" windowHeight="16940" xr2:uid="{5B8FBCEC-8CE4-C24B-9B42-841DBEEE8CF1}"/>
+    <workbookView xWindow="10380" yWindow="500" windowWidth="28560" windowHeight="26640" activeTab="1" xr2:uid="{5B8FBCEC-8CE4-C24B-9B42-841DBEEE8CF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>Supplementary Table 1</t>
   </si>
@@ -256,6 +257,30 @@
       </rPr>
       <t xml:space="preserve">-index </t>
     </r>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>kernel</t>
+  </si>
+  <si>
+    <t>nonlinear_regression</t>
+  </si>
+  <si>
+    <t>sparse_linear_regression</t>
+  </si>
+  <si>
+    <t>PLS_PC_Regression</t>
+  </si>
+  <si>
+    <t>Ensemble</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -437,68 +462,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B2349A-B3D0-9345-8978-1219D448EC5C}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -843,25 +868,25 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="18" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="17" thickBot="1">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="19">
         <v>0.58299999999999996</v>
       </c>
       <c r="D4">
@@ -869,13 +894,13 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="25" thickBot="1">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="19">
         <v>0.55900000000000005</v>
       </c>
       <c r="D5">
@@ -883,13 +908,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="25" thickBot="1">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="19">
         <v>0.55300000000000005</v>
       </c>
       <c r="D6">
@@ -897,13 +922,13 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="24">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="19">
         <v>0.54900000000000004</v>
       </c>
       <c r="D7">
@@ -911,20 +936,20 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:4" ht="25" thickBot="1">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>1</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="19">
         <v>0.57699999999999996</v>
       </c>
       <c r="D9">
@@ -932,13 +957,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="25" thickBot="1">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>2</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="19">
         <v>0.56899999999999995</v>
       </c>
       <c r="D10">
@@ -946,13 +971,13 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="25" thickBot="1">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>3</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="19">
         <v>0.56499999999999995</v>
       </c>
       <c r="D11">
@@ -960,13 +985,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="25" thickBot="1">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>4</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="19">
         <v>0.56399999999999995</v>
       </c>
       <c r="D12">
@@ -974,13 +999,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="25" thickBot="1">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>5</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="19">
         <v>0.55900000000000005</v>
       </c>
       <c r="D13">
@@ -988,13 +1013,13 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="25" thickBot="1">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>6</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="19">
         <v>0.55100000000000005</v>
       </c>
       <c r="D14">
@@ -1002,13 +1027,13 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="37" thickBot="1">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>7</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="19">
         <v>0.54800000000000004</v>
       </c>
       <c r="D15">
@@ -1016,13 +1041,13 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="25" thickBot="1">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>8</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="19">
         <v>0.54800000000000004</v>
       </c>
       <c r="D16">
@@ -1030,13 +1055,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="25" thickBot="1">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>9</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="19">
         <v>0.54400000000000004</v>
       </c>
       <c r="D17">
@@ -1044,13 +1069,13 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="25" thickBot="1">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>10</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="19">
         <v>0.53800000000000003</v>
       </c>
       <c r="D18">
@@ -1058,13 +1083,13 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="36">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>11</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="19">
         <v>0.52400000000000002</v>
       </c>
       <c r="D19">
@@ -1072,20 +1097,20 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" spans="1:4" ht="17" thickBot="1">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>1</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="19">
         <v>0.56399999999999995</v>
       </c>
       <c r="D21">
@@ -1093,13 +1118,13 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" thickBot="1">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>2</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <v>0.56399999999999995</v>
       </c>
       <c r="D22">
@@ -1107,13 +1132,13 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="25" thickBot="1">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>3</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23" s="19">
         <v>0.56399999999999995</v>
       </c>
       <c r="D23">
@@ -1121,13 +1146,13 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="25" thickBot="1">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>4</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="19">
         <v>0.55100000000000005</v>
       </c>
       <c r="D24">
@@ -1135,13 +1160,13 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="37" thickBot="1">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>5</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="19">
         <v>0.53900000000000003</v>
       </c>
       <c r="D25">
@@ -1149,13 +1174,13 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="25" thickBot="1">
-      <c r="A26" s="7">
+      <c r="A26" s="6">
         <v>6</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="19">
         <v>0.53900000000000003</v>
       </c>
       <c r="D26">
@@ -1163,13 +1188,13 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" thickBot="1">
-      <c r="A27" s="7">
+      <c r="A27" s="6">
         <v>7</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="19">
         <v>0.53200000000000003</v>
       </c>
       <c r="D27">
@@ -1177,13 +1202,13 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="25" thickBot="1">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>8</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="19">
         <v>0.53100000000000003</v>
       </c>
       <c r="D28">
@@ -1191,13 +1216,13 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="25" thickBot="1">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>9</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="19">
         <v>0.53100000000000003</v>
       </c>
       <c r="D29">
@@ -1205,13 +1230,13 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="25" thickBot="1">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>10</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <v>0.53100000000000003</v>
       </c>
       <c r="D30">
@@ -1219,13 +1244,13 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="25" thickBot="1">
-      <c r="A31" s="7">
+      <c r="A31" s="6">
         <v>11</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="19">
         <v>0.52700000000000002</v>
       </c>
       <c r="D31">
@@ -1233,13 +1258,13 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="25" thickBot="1">
-      <c r="A32" s="7">
+      <c r="A32" s="6">
         <v>12</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="25">
+      <c r="C32" s="19">
         <v>0.51900000000000002</v>
       </c>
       <c r="D32">
@@ -1247,13 +1272,13 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" thickBot="1">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>13</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="25">
+      <c r="C33" s="19">
         <v>0.51700000000000002</v>
       </c>
       <c r="D33">
@@ -1261,13 +1286,13 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="24">
-      <c r="A34" s="7">
+      <c r="A34" s="6">
         <v>14</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="19">
         <v>0.48499999999999999</v>
       </c>
       <c r="D34">
@@ -1275,20 +1300,20 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:4" ht="25" thickBot="1">
-      <c r="A36" s="7">
+      <c r="A36" s="6">
         <v>1</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="25">
+      <c r="C36" s="19">
         <v>0.56200000000000006</v>
       </c>
       <c r="D36">
@@ -1296,13 +1321,13 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="37" thickBot="1">
-      <c r="A37" s="7">
+      <c r="A37" s="6">
         <v>2</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="25">
+      <c r="C37" s="19">
         <v>0.54300000000000004</v>
       </c>
       <c r="D37">
@@ -1310,13 +1335,13 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" thickBot="1">
-      <c r="A38" s="7">
+      <c r="A38" s="6">
         <v>3</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="25">
+      <c r="C38" s="19">
         <v>0.53500000000000003</v>
       </c>
       <c r="D38">
@@ -1324,13 +1349,13 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="24">
-      <c r="A39" s="7">
+      <c r="A39" s="6">
         <v>4</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="25">
+      <c r="C39" s="19">
         <v>0.52400000000000002</v>
       </c>
       <c r="D39">
@@ -1338,20 +1363,20 @@
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="16"/>
     </row>
     <row r="41" spans="1:4" ht="25" thickBot="1">
-      <c r="A41" s="7">
+      <c r="A41" s="6">
         <v>1</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="25">
+      <c r="C41" s="19">
         <v>0.56200000000000006</v>
       </c>
       <c r="D41">
@@ -1359,13 +1384,13 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="25" thickBot="1">
-      <c r="A42" s="7">
+      <c r="A42" s="6">
         <v>2</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="25">
+      <c r="C42" s="19">
         <v>0.55600000000000005</v>
       </c>
       <c r="D42">
@@ -1373,13 +1398,13 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="37" thickBot="1">
-      <c r="A43" s="7">
+      <c r="A43" s="6">
         <v>3</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="25">
+      <c r="C43" s="19">
         <v>0.55400000000000005</v>
       </c>
       <c r="D43">
@@ -1387,13 +1412,13 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="25" thickBot="1">
-      <c r="A44" s="7">
+      <c r="A44" s="6">
         <v>4</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="25">
+      <c r="C44" s="19">
         <v>0.51700000000000002</v>
       </c>
       <c r="D44">
@@ -1401,13 +1426,13 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="24">
-      <c r="A45" s="7">
+      <c r="A45" s="6">
         <v>5</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="25">
+      <c r="C45" s="19">
         <v>0.50600000000000001</v>
       </c>
       <c r="D45">
@@ -1415,20 +1440,20 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="23"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="17"/>
     </row>
     <row r="47" spans="1:4" ht="25" thickBot="1">
-      <c r="A47" s="7">
+      <c r="A47" s="6">
         <v>1</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="25">
+      <c r="C47" s="19">
         <v>0.56999999999999995</v>
       </c>
       <c r="D47">
@@ -1436,13 +1461,13 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="25" thickBot="1">
-      <c r="A48" s="7">
+      <c r="A48" s="6">
         <v>2</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="25">
+      <c r="C48" s="19">
         <v>0.55300000000000005</v>
       </c>
       <c r="D48">
@@ -1450,13 +1475,13 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="37" thickBot="1">
-      <c r="A49" s="7">
+      <c r="A49" s="6">
         <v>3</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="25">
+      <c r="C49" s="19">
         <v>0.55300000000000005</v>
       </c>
       <c r="D49">
@@ -1464,13 +1489,13 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="17" thickBot="1">
-      <c r="A50" s="7">
+      <c r="A50" s="6">
         <v>4</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="25">
+      <c r="C50" s="19">
         <v>0.53100000000000003</v>
       </c>
       <c r="D50">
@@ -1478,13 +1503,13 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="25" thickBot="1">
-      <c r="A51" s="7">
+      <c r="A51" s="6">
         <v>5</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="25">
+      <c r="C51" s="19">
         <v>0.52800000000000002</v>
       </c>
       <c r="D51">
@@ -1492,13 +1517,13 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="24">
-      <c r="A52" s="7">
+      <c r="A52" s="6">
         <v>6</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="25">
+      <c r="C52" s="19">
         <v>0.52100000000000002</v>
       </c>
       <c r="D52">
@@ -1507,13 +1532,526 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A46:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBED852F-7AD4-BC47-8E35-9EEF83660444}">
+  <dimension ref="A1:C45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="19">
+        <v>0.58299999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="19">
+        <v>0.55900000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="19">
+        <v>0.54900000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0.57699999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.56899999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="19">
+        <v>0.56499999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="19">
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="19">
+        <v>0.55900000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="19">
+        <v>0.54800000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="19">
+        <v>0.54800000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="19">
+        <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="19">
+        <v>0.53800000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="19">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="19">
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="19">
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="19">
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="19">
+        <v>0.53900000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="19">
+        <v>0.53900000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="19">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="19">
+        <v>0.53100000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="19">
+        <v>0.53100000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.53100000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="19">
+        <v>0.52700000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="19">
+        <v>0.51900000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="19">
+        <v>0.51700000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="19">
+        <v>0.48499999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="19">
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="19">
+        <v>0.54300000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="19">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="19">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="19">
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="19">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="19">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="19">
+        <v>0.51700000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="19">
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="19">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="19">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="19">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="19">
+        <v>0.53100000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="19">
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="19">
+        <v>0.52100000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>